<commit_message>
alpha 0.1.10 Regular Update
Update: `UI\style.css`, `UI\main.html`, `UI\api.js`,  `UI\main.js`, `UI\locale.json`, `main.py`, `readfile.py`, `Restaurants.xlsx`
Removed: `reastaurants.py` (No longer required)

Description: Add analyze() for JavaScript to retrieve sheet data; Fix the dropdown's option is unclickable when open through eel; Add 3rd and last part for the query.
</commit_message>
<xml_diff>
--- a/Restaurants.xlsx
+++ b/Restaurants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielHo\Documents\GitHub-Repos\what-2-eat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57324E86-60DD-47FC-9235-8C8804704C06}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B008EB5D-5A31-4F51-B5BA-E4AE1D1FD6B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>*</t>
-  </si>
-  <si>
-    <t>11:30~14:00/16:30~22:00</t>
   </si>
   <si>
     <t>JJ's POKE &amp; CAFE</t>
@@ -349,6 +346,10 @@
   </si>
   <si>
     <t>鱷吐司（公館店）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>11:30-14:00/16:30-22:00</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -734,7 +735,7 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -792,10 +793,10 @@
         <v>12</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -803,7 +804,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>14</v>
@@ -815,7 +816,7 @@
         <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -827,10 +828,10 @@
         <v>4.2</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -838,10 +839,10 @@
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>15</v>
@@ -850,7 +851,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -861,10 +862,10 @@
         <v>4</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -872,10 +873,10 @@
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>15</v>
@@ -884,7 +885,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3"/>
       <c r="I4" s="2"/>
@@ -895,30 +896,30 @@
         <v>4.2</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="1"/>
@@ -929,21 +930,21 @@
         <v>4</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>15</v>
@@ -952,7 +953,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
@@ -964,21 +965,21 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N6" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>15</v>
@@ -987,7 +988,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -999,21 +1000,21 @@
         <v>3.9</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>15</v>
@@ -1022,7 +1023,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1034,21 +1035,21 @@
         <v>3.3</v>
       </c>
       <c r="N8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O8" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="O8" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>15</v>
@@ -1057,7 +1058,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1069,21 +1070,21 @@
         <v>3.9</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>15</v>
@@ -1092,7 +1093,7 @@
         <v>16</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1104,10 +1105,10 @@
         <v>3.9</v>
       </c>
       <c r="N10" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1115,10 +1116,10 @@
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
@@ -1127,7 +1128,7 @@
         <v>16</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3"/>
@@ -1139,30 +1140,30 @@
         <v>4.8</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1173,30 +1174,30 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N12" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="O12" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -1207,10 +1208,10 @@
         <v>4</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1218,10 +1219,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>15</v>
@@ -1230,7 +1231,7 @@
         <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1241,30 +1242,30 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="N14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="O14" s="5" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1275,30 +1276,30 @@
         <v>4.5</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G16" s="3"/>
       <c r="I16" s="2"/>
@@ -1309,21 +1310,21 @@
         <v>4.3</v>
       </c>
       <c r="N16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="O16" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="O16" s="5" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>15</v>
@@ -1332,7 +1333,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
@@ -1344,10 +1345,10 @@
         <v>4.7</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
beta 0.2.1 Regular Update
Update: `UI\style.css`, `UI\main.html`,  `UI\main.js`, `UI\favicon.ico`, `UI\locale.json`, `README.md`, `main.py`, `readfile.py`, `Restaurants.xlsx`

Description: Query function is available now.
</commit_message>
<xml_diff>
--- a/Restaurants.xlsx
+++ b/Restaurants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanielHo\Documents\GitHub-Repos\what-2-eat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B008EB5D-5A31-4F51-B5BA-E4AE1D1FD6B8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8C1EB1-6742-4FA1-BDDE-3724B378948E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="103">
   <si>
     <t>Type</t>
   </si>
@@ -350,6 +350,10 @@
   </si>
   <si>
     <t>11:30-14:00/16:30-22:00</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distance</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -732,10 +736,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O1000"/>
+  <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -752,7 +756,7 @@
     <col min="16" max="16384" width="8.796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -798,8 +802,11 @@
       <c r="O1" s="5" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P1" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -833,8 +840,11 @@
       <c r="O2" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -867,8 +877,11 @@
       <c r="O3" s="5" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="5">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -901,8 +914,11 @@
       <c r="O4" s="5" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P4" s="5">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -935,8 +951,11 @@
       <c r="O5" s="5" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P5" s="5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -970,8 +989,11 @@
       <c r="O6" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P6" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
@@ -1005,8 +1027,11 @@
       <c r="O7" s="5" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P7" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
@@ -1040,8 +1065,11 @@
       <c r="O8" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P8" s="5">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>35</v>
       </c>
@@ -1075,8 +1103,11 @@
       <c r="O9" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P9" s="5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1110,8 +1141,11 @@
       <c r="O10" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1145,8 +1179,11 @@
       <c r="O11" s="5" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P11" s="5">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1179,8 +1216,11 @@
       <c r="O12" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1213,8 +1253,11 @@
       <c r="O13" s="5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P13" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1247,8 +1290,11 @@
       <c r="O14" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1281,8 +1327,11 @@
       <c r="O15" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P15" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1315,8 +1364,11 @@
       <c r="O16" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P16" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1350,8 +1402,11 @@
       <c r="O17" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P17" s="5">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1366,7 +1421,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1381,7 +1436,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1396,7 +1451,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="1"/>
@@ -1411,7 +1466,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
@@ -1426,7 +1481,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
@@ -1441,7 +1496,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="2"/>
     </row>
-    <row r="24" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1456,7 +1511,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="2"/>
     </row>
-    <row r="25" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="3"/>
@@ -1471,7 +1526,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1486,7 +1541,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1499,7 +1554,7 @@
       <c r="J27" s="2"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1511,7 +1566,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1523,7 +1578,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1535,7 +1590,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1547,7 +1602,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>

</xml_diff>